<commit_message>
Small layout changes requested by Han
</commit_message>
<xml_diff>
--- a/Altium/DTCP v1.2/Project Outputs for DTCP v1.2/Assembly/BOM/Bill of Materials-DTCP v1.2.xlsx
+++ b/Altium/DTCP v1.2/Project Outputs for DTCP v1.2/Assembly/BOM/Bill of Materials-DTCP v1.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\AppData\Local\TempReleases\Snapshot\5\Assembly\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\AppData\Local\TempReleases\Snapshot\1\Assembly\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF06B2EB-D26E-4EDE-A4B7-60E84F227880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3A9BDA6-F640-493F-828A-1512321D68FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{A88852C5-88AF-425A-8C11-B5F1E4FF1E94}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{29F61425-8799-46F9-95B9-AEE497066B50}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-DTCP v1.2" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="301">
   <si>
     <t>Comment</t>
   </si>
@@ -224,7 +224,7 @@
     <t>VJ0603D471KXXAJ</t>
   </si>
   <si>
-    <t>C18, C43, C44, C45, C46, C56, C57, C58, C59, C60</t>
+    <t>C18, C43, C45, C59</t>
   </si>
   <si>
     <t>CAPC1608X92X38LL15T08</t>
@@ -449,49 +449,34 @@
     <t>L4</t>
   </si>
   <si>
+    <t>LQW2BHN68NJ03L</t>
+  </si>
+  <si>
+    <t>Wire Wound RF Inductor 68nH ±5% 460mA 0.23Ω 0805 (2015)</t>
+  </si>
+  <si>
+    <t>L5, L6, L7</t>
+  </si>
+  <si>
+    <t>FP-LQW2BHN_03-MFG</t>
+  </si>
+  <si>
+    <t>CMP-06042-008671-1</t>
+  </si>
+  <si>
     <t>1812PS-333_R_</t>
   </si>
   <si>
-    <t>1812PS-333_R_Coilcraft, 1812PS-333_R_ Coilcraft</t>
-  </si>
-  <si>
-    <t>L5, L6, L10</t>
+    <t>1812PS-333_R_ Coilcraft</t>
+  </si>
+  <si>
+    <t>L10</t>
   </si>
   <si>
     <t>FP-1812PS-MFG</t>
   </si>
   <si>
     <t>CMP-11268-000188-1</t>
-  </si>
-  <si>
-    <t>LQG18HHR10J00D</t>
-  </si>
-  <si>
-    <t>Multilayer type Inductor for Automotive 100nH ±5% 0.9Ω 300mA 0603</t>
-  </si>
-  <si>
-    <t>L7, L8, L9, L11, L12</t>
-  </si>
-  <si>
-    <t>FP-LQG18HH_00-MFG</t>
-  </si>
-  <si>
-    <t>CMP-06042-004589-1</t>
-  </si>
-  <si>
-    <t>LQG18HH82NJ00D</t>
-  </si>
-  <si>
-    <t>Multilayer type Inductor for Automotive 82nH ±5% 0.85Ω 300mA 0603</t>
-  </si>
-  <si>
-    <t>L13</t>
-  </si>
-  <si>
-    <t>FP-LQG18HH_00-IPC_B</t>
-  </si>
-  <si>
-    <t>CMP-06042-003651-1</t>
   </si>
   <si>
     <t>MLZ2012M1R0HTD25</t>
@@ -1352,8 +1337,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7235AF0-F135-46B6-9DF6-BCCDBF03738D}">
-  <dimension ref="A1:F65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51EE474-5DEF-4899-B876-2FC39B668987}">
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1619,7 +1604,7 @@
         <v>63</v>
       </c>
       <c r="F13" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1979,7 +1964,7 @@
         <v>145</v>
       </c>
       <c r="F31" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1999,7 +1984,7 @@
         <v>150</v>
       </c>
       <c r="F32" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,7 +2004,7 @@
         <v>155</v>
       </c>
       <c r="F33" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,7 +2024,7 @@
         <v>160</v>
       </c>
       <c r="F34" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2056,30 +2041,30 @@
         <v>164</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F35" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="F36" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2099,7 +2084,7 @@
         <v>174</v>
       </c>
       <c r="F37" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2119,7 +2104,7 @@
         <v>179</v>
       </c>
       <c r="F38" s="1">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2139,7 +2124,7 @@
         <v>184</v>
       </c>
       <c r="F39" s="1">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,27 +2132,27 @@
         <v>185</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="F40" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>191</v>
@@ -2179,7 +2164,7 @@
         <v>193</v>
       </c>
       <c r="F41" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2187,33 +2172,33 @@
         <v>194</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="F42" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>201</v>
@@ -2239,7 +2224,7 @@
         <v>206</v>
       </c>
       <c r="F44" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2259,7 +2244,7 @@
         <v>211</v>
       </c>
       <c r="F45" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2267,16 +2252,16 @@
         <v>212</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="F46" s="1">
         <v>4</v>
@@ -2284,42 +2269,42 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="F47" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>224</v>
       </c>
       <c r="F48" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2339,7 +2324,7 @@
         <v>229</v>
       </c>
       <c r="F49" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2379,7 +2364,7 @@
         <v>239</v>
       </c>
       <c r="F51" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2399,7 +2384,7 @@
         <v>244</v>
       </c>
       <c r="F52" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2436,7 +2421,7 @@
         <v>253</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F54" s="1">
         <v>1</v>
@@ -2444,22 +2429,22 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="F55" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2499,7 +2484,7 @@
         <v>268</v>
       </c>
       <c r="F57" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2536,7 +2521,7 @@
         <v>277</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
@@ -2544,19 +2529,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>282</v>
-      </c>
       <c r="E60" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F60" s="1">
         <v>1</v>
@@ -2564,19 +2549,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="F61" s="1">
         <v>1</v>
@@ -2596,7 +2581,7 @@
         <v>290</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F62" s="1">
         <v>1</v>
@@ -2604,19 +2589,19 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="F63" s="1">
         <v>1</v>
@@ -2639,26 +2624,6 @@
         <v>300</v>
       </c>
       <c r="F64" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="F65" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>